<commit_message>
Updates to the SVM as well as mushrooms and alike - also PASSED the QUIZ - 81%
</commit_message>
<xml_diff>
--- a/4_Applied ML with Python/Models.xlsx
+++ b/4_Applied ML with Python/Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FF179D-9EF4-43BE-9E2C-E72E833D09B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0533649-DB53-4ECA-B322-CEDAD5094416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Sr. #</t>
   </si>
@@ -176,13 +176,25 @@
   </si>
   <si>
     <t>clf = SVC(kernel = 'linear', C=1.0).fit(X_train, y_train)</t>
+  </si>
+  <si>
+    <t>Kernelized SVM</t>
+  </si>
+  <si>
+    <t>svm = SVC(kernel='rbf', C=10, gamma=0.1).fit(X, y)</t>
+  </si>
+  <si>
+    <t>C &amp; gamma</t>
+  </si>
+  <si>
+    <t>Better C and gamma means more accurate model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,12 +205,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF002060"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -335,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -343,88 +349,85 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -749,10 +752,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G22"/>
+  <dimension ref="B1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -769,272 +772,299 @@
   <sheetData>
     <row r="1" spans="2:7" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:7" s="29" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="2:7" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="B4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="25" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="14"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="22" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="14"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="22" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="26" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="22" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>4</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="4" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>5</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="22" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>6</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="11"/>
+      <c r="F19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <v>7</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="B21" s="19"/>
-      <c r="C21" s="15" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="30" t="s">
+      <c r="E21" s="20"/>
+      <c r="F21" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="B22" s="2">
+        <v>8</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>